<commit_message>
Update excels and listings
</commit_message>
<xml_diff>
--- a/excels/Dover.xlsx
+++ b/excels/Dover.xlsx
@@ -10,13 +10,16 @@
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Listing_0" sheetId="2" r:id="rId2"/>
     <sheet name="Listing_1" sheetId="3" r:id="rId3"/>
+    <sheet name="Listing_2" sheetId="4" r:id="rId4"/>
+    <sheet name="Listing_3" sheetId="5" r:id="rId5"/>
+    <sheet name="Listing_4" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>Mean Comparable Airbnb Turnover</t>
   </si>
@@ -33,6 +36,9 @@
     <t>Nb Nearby Airbnbs</t>
   </si>
   <si>
+    <t>Mean Turnover / 2</t>
+  </si>
+  <si>
     <t>60% of (Mean Turnover - Rent)</t>
   </si>
   <si>
@@ -42,10 +48,19 @@
     <t>Listing</t>
   </si>
   <si>
-    <t>https://www.zoopla.co.uk/to-rent/details/43370466/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
-  </si>
-  <si>
-    <t>https://www.zoopla.co.uk/to-rent/details/63851631/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
+    <t>https://www.zoopla.co.uk/to-rent/details/63918717/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
+  </si>
+  <si>
+    <t>https://www.zoopla.co.uk/to-rent/details/63531878/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
+  </si>
+  <si>
+    <t>https://www.zoopla.co.uk/to-rent/details/63770336/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
+  </si>
+  <si>
+    <t>https://www.zoopla.co.uk/to-rent/details/63917670/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
+  </si>
+  <si>
+    <t>https://www.openrent.co.uk/1619751</t>
   </si>
   <si>
     <t>Airbnb URL</t>
@@ -66,16 +81,16 @@
     <t>Daily Income</t>
   </si>
   <si>
-    <t>Mean Daily Income</t>
-  </si>
-  <si>
-    <t>Median Daily Income</t>
+    <t>Mean Monthly Income</t>
+  </si>
+  <si>
+    <t>Median Monthly Income</t>
   </si>
   <si>
     <t>Distance (km)</t>
   </si>
   <si>
-    <t>Listing Rent</t>
+    <t>Listing Daily Rent</t>
   </si>
   <si>
     <t>Listing Bedrooms</t>
@@ -87,28 +102,46 @@
     <t>Listing URL</t>
   </si>
   <si>
-    <t>https://www.airbnb.com/rooms/15876160</t>
-  </si>
-  <si>
-    <t>https://www.airbnb.com/rooms/52989745</t>
-  </si>
-  <si>
-    <t>15876160</t>
-  </si>
-  <si>
-    <t>52989745</t>
-  </si>
-  <si>
-    <t>https://www.airbnb.com/rooms/12591307</t>
-  </si>
-  <si>
-    <t>https://www.airbnb.com/rooms/48410970</t>
-  </si>
-  <si>
-    <t>12591307</t>
-  </si>
-  <si>
-    <t>48410970</t>
+    <t>https://www.airbnb.com/rooms/24175680</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/30889197</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/51550912</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/618725391273418153</t>
+  </si>
+  <si>
+    <t>24175680</t>
+  </si>
+  <si>
+    <t>30889197</t>
+  </si>
+  <si>
+    <t>51550912</t>
+  </si>
+  <si>
+    <t>618725391273418153</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/627260390537024013</t>
+  </si>
+  <si>
+    <t>627260390537024013</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/51879359</t>
+  </si>
+  <si>
+    <t>51879359</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/35507556</t>
+  </si>
+  <si>
+    <t>35507556</t>
   </si>
 </sst>
 </file>
@@ -479,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,9 +527,9 @@
     <col min="8" max="8" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -519,63 +552,162 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1592.584315318976</v>
+        <v>2109.913629484222</v>
       </c>
       <c r="C2">
-        <v>1592.584315318976</v>
+        <v>1900.586950682596</v>
       </c>
       <c r="D2">
-        <v>750</v>
+        <v>895</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>505.5505891913857</v>
+        <v>1054.956814742111</v>
       </c>
       <c r="H2">
-        <v>505.5505891913857</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>728.9481776905334</v>
+      </c>
+      <c r="I2">
+        <v>603.3521704095575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2652.397399431126</v>
+        <v>6788.168210976479</v>
       </c>
       <c r="C3">
-        <v>2652.397399431126</v>
+        <v>6788.168210976479</v>
       </c>
       <c r="D3">
-        <v>1100</v>
+        <v>1450</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3394.084105488239</v>
+      </c>
+      <c r="H3">
+        <v>3202.900926585887</v>
+      </c>
+      <c r="I3">
+        <v>3202.900926585887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>931.4384396586755</v>
-      </c>
-      <c r="H3">
-        <v>931.4384396586755</v>
+      <c r="B4">
+        <v>1921.357951161406</v>
+      </c>
+      <c r="C4">
+        <v>1921.357951161406</v>
+      </c>
+      <c r="D4">
+        <v>850</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>960.6789755807029</v>
+      </c>
+      <c r="H4">
+        <v>642.8147706968434</v>
+      </c>
+      <c r="I4">
+        <v>642.8147706968434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="C5">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="D5">
+        <v>994.9999999999999</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1814.054284012593</v>
+      </c>
+      <c r="H5">
+        <v>1579.865140815111</v>
+      </c>
+      <c r="I5">
+        <v>1579.865140815111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="C6">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="D6">
+        <v>850</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1814.054284012593</v>
+      </c>
+      <c r="H6">
+        <v>1666.865140815111</v>
+      </c>
+      <c r="I6">
+        <v>1666.865140815111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -583,7 +715,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -606,125 +738,207 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>118.5714285714286</v>
+        <v>111.6666666666667</v>
       </c>
       <c r="E2">
-        <v>36.88172043010752</v>
+        <v>69.03161802355351</v>
       </c>
       <c r="F2">
-        <v>37.38317757009346</v>
+        <v>65.89874925550923</v>
       </c>
       <c r="G2">
-        <v>53.08614384396587</v>
+        <v>2109.913629484222</v>
       </c>
       <c r="H2">
-        <v>53.08614384396587</v>
+        <v>1900.586950682596</v>
       </c>
       <c r="I2">
-        <v>0.4818111537939595</v>
+        <v>0.4102767204892596</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>29.83333333333333</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>187.2857142857143</v>
+        <v>160.1818181818182</v>
       </c>
       <c r="E3">
-        <v>50.44546850998464</v>
+        <v>73.33403155983802</v>
       </c>
       <c r="F3">
-        <v>68.78911011783828</v>
+        <v>101.0746268656717</v>
       </c>
       <c r="G3">
-        <v>53.08614384396587</v>
+        <v>2109.913629484222</v>
       </c>
       <c r="H3">
-        <v>53.08614384396587</v>
+        <v>1900.586950682596</v>
       </c>
       <c r="I3">
-        <v>0.4978861493377521</v>
+        <v>0.1868066645272088</v>
       </c>
       <c r="J3">
-        <v>25</v>
+        <v>29.83333333333333</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>123.75</v>
+      </c>
+      <c r="E4">
+        <v>49.75742447516642</v>
+      </c>
+      <c r="F4">
+        <v>53.54139368671829</v>
+      </c>
+      <c r="G4">
+        <v>2109.913629484222</v>
+      </c>
+      <c r="H4">
+        <v>1900.586950682596</v>
+      </c>
+      <c r="I4">
+        <v>0.4963474877610286</v>
+      </c>
+      <c r="J4">
+        <v>29.83333333333333</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="E5">
+        <v>71.03225806451613</v>
+      </c>
+      <c r="F5">
+        <v>60.80704745666383</v>
+      </c>
+      <c r="G5">
+        <v>2109.913629484222</v>
+      </c>
+      <c r="H5">
+        <v>1900.586950682596</v>
+      </c>
+      <c r="I5">
+        <v>0.2574099493720388</v>
+      </c>
+      <c r="J5">
+        <v>29.83333333333333</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -733,6 +947,10 @@
     <hyperlink ref="M2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
     <hyperlink ref="M3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="M4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
+    <hyperlink ref="M5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -740,7 +958,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -763,133 +981,432 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>158.4285714285714</v>
+        <v>858</v>
       </c>
       <c r="E2">
-        <v>64.50076804915514</v>
+        <v>30.51075268817204</v>
       </c>
       <c r="F2">
-        <v>88.37870784234052</v>
+        <v>226.272273699216</v>
       </c>
       <c r="G2">
-        <v>88.4132466477042</v>
+        <v>6788.168210976479</v>
       </c>
       <c r="H2">
-        <v>88.4132466477042</v>
+        <v>6788.168210976479</v>
       </c>
       <c r="I2">
-        <v>0.3028644921614171</v>
+        <v>0.183959480597031</v>
       </c>
       <c r="J2">
-        <v>36.66666666666666</v>
+        <v>48.33333333333334</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>126.5714285714286</v>
-      </c>
-      <c r="E3">
-        <v>80.3379416282642</v>
-      </c>
-      <c r="F3">
-        <v>88.44778545306787</v>
-      </c>
-      <c r="G3">
-        <v>88.4132466477042</v>
-      </c>
-      <c r="H3">
-        <v>88.4132466477042</v>
-      </c>
-      <c r="I3">
-        <v>0.3629573187246821</v>
-      </c>
-      <c r="J3">
-        <v>36.66666666666666</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>156.0909090909091</v>
+      </c>
+      <c r="E2">
+        <v>47.8289810547875</v>
+      </c>
+      <c r="F2">
+        <v>64.04526503871352</v>
+      </c>
+      <c r="G2">
+        <v>1921.357951161406</v>
+      </c>
+      <c r="H2">
+        <v>1921.357951161406</v>
+      </c>
+      <c r="I2">
+        <v>0.1334581662477377</v>
+      </c>
+      <c r="J2">
+        <v>28.33333333333333</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>191.7142857142857</v>
+      </c>
+      <c r="E2">
+        <v>72.73233486943165</v>
+      </c>
+      <c r="F2">
+        <v>120.9369522675062</v>
+      </c>
+      <c r="G2">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="H2">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="I2">
+        <v>0.2311457247865123</v>
+      </c>
+      <c r="J2">
+        <v>33.16666666666666</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>191.7142857142857</v>
+      </c>
+      <c r="E2">
+        <v>72.73233486943165</v>
+      </c>
+      <c r="F2">
+        <v>120.9369522675062</v>
+      </c>
+      <c r="G2">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="H2">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="I2">
+        <v>0.4835642264939813</v>
+      </c>
+      <c r="J2">
+        <v>28.33333333333333</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update excels and listings, debug true
</commit_message>
<xml_diff>
--- a/excels/Dover.xlsx
+++ b/excels/Dover.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="44">
   <si>
     <t>Mean Comparable Airbnb Turnover</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Listing</t>
   </si>
   <si>
-    <t>https://www.zoopla.co.uk/to-rent/details/63918717/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
+    <t>https://www.zoopla.co.uk/to-rent/details/63993388/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
   </si>
   <si>
     <t>https://www.zoopla.co.uk/to-rent/details/63531878/?search_identifier=0a18dc707f181723ef9e9bbd03981c3b</t>
@@ -63,6 +63,9 @@
     <t>https://www.openrent.co.uk/1619751</t>
   </si>
   <si>
+    <t>Airbnb link is active</t>
+  </si>
+  <si>
     <t>Airbnb URL</t>
   </si>
   <si>
@@ -102,28 +105,34 @@
     <t>Listing URL</t>
   </si>
   <si>
-    <t>https://www.airbnb.com/rooms/24175680</t>
-  </si>
-  <si>
-    <t>https://www.airbnb.com/rooms/30889197</t>
-  </si>
-  <si>
-    <t>https://www.airbnb.com/rooms/51550912</t>
-  </si>
-  <si>
-    <t>https://www.airbnb.com/rooms/618725391273418153</t>
-  </si>
-  <si>
-    <t>24175680</t>
-  </si>
-  <si>
-    <t>30889197</t>
-  </si>
-  <si>
-    <t>51550912</t>
-  </si>
-  <si>
-    <t>618725391273418153</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/40932692</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/43528626</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/51467691</t>
+  </si>
+  <si>
+    <t>https://www.airbnb.com/rooms/53018851</t>
+  </si>
+  <si>
+    <t>40932692</t>
+  </si>
+  <si>
+    <t>43528626</t>
+  </si>
+  <si>
+    <t>51467691</t>
+  </si>
+  <si>
+    <t>53018851</t>
   </si>
   <si>
     <t>https://www.airbnb.com/rooms/627260390537024013</t>
@@ -561,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2109.913629484222</v>
+        <v>4823.98945779303</v>
       </c>
       <c r="C2">
-        <v>1900.586950682596</v>
+        <v>5258.521847420001</v>
       </c>
       <c r="D2">
-        <v>895</v>
+        <v>1500</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -576,13 +585,13 @@
         <v>4</v>
       </c>
       <c r="G2">
-        <v>1054.956814742111</v>
+        <v>2411.994728896515</v>
       </c>
       <c r="H2">
-        <v>728.9481776905334</v>
+        <v>1994.393674675818</v>
       </c>
       <c r="I2">
-        <v>603.3521704095575</v>
+        <v>2255.113108452001</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -625,7 +634,7 @@
         <v>1921.357951161406</v>
       </c>
       <c r="D4">
-        <v>850</v>
+        <v>830</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -637,10 +646,10 @@
         <v>960.6789755807029</v>
       </c>
       <c r="H4">
-        <v>642.8147706968434</v>
+        <v>654.8147706968434</v>
       </c>
       <c r="I4">
-        <v>642.8147706968434</v>
+        <v>654.8147706968434</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -715,17 +724,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
@@ -733,10 +742,10 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -776,181 +785,196 @@
       <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>227.1666666666666</v>
+      </c>
+      <c r="F2">
+        <v>73.33589349718382</v>
+      </c>
+      <c r="G2">
+        <v>145.7351598173516</v>
+      </c>
+      <c r="H2">
+        <v>4823.98945779303</v>
+      </c>
+      <c r="I2">
+        <v>5258.521847420001</v>
+      </c>
+      <c r="J2">
+        <v>0.2980403688985191</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2">
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>111.6666666666667</v>
-      </c>
-      <c r="E2">
-        <v>69.03161802355351</v>
-      </c>
-      <c r="F2">
-        <v>65.89874925550923</v>
-      </c>
-      <c r="G2">
-        <v>2109.913629484222</v>
-      </c>
-      <c r="H2">
-        <v>1900.586950682596</v>
-      </c>
-      <c r="I2">
-        <v>0.4102767204892596</v>
-      </c>
-      <c r="J2">
-        <v>29.83333333333333</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
+      <c r="E3">
+        <v>461.8181818181818</v>
+      </c>
+      <c r="F3">
+        <v>51.2467997951869</v>
+      </c>
+      <c r="G3">
+        <v>204.8329633439818</v>
+      </c>
+      <c r="H3">
+        <v>4823.98945779303</v>
+      </c>
+      <c r="I3">
+        <v>5258.521847420001</v>
+      </c>
+      <c r="J3">
+        <v>0.3604957192869395</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>171.8571428571429</v>
+      </c>
+      <c r="F4">
+        <v>54.69470046082948</v>
+      </c>
+      <c r="G4">
+        <v>81.60469667318985</v>
+      </c>
+      <c r="H4">
+        <v>4823.98945779303</v>
+      </c>
+      <c r="I4">
+        <v>5258.521847420001</v>
+      </c>
+      <c r="J4">
+        <v>0.1866178748004681</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>160.1818181818182</v>
-      </c>
-      <c r="E3">
-        <v>73.33403155983802</v>
-      </c>
-      <c r="F3">
-        <v>101.0746268656717</v>
-      </c>
-      <c r="G3">
-        <v>2109.913629484222</v>
-      </c>
-      <c r="H3">
-        <v>1900.586950682596</v>
-      </c>
-      <c r="I3">
-        <v>0.1868066645272088</v>
-      </c>
-      <c r="J3">
-        <v>29.83333333333333</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
+      <c r="E5">
+        <v>510</v>
+      </c>
+      <c r="F5">
+        <v>47.83130847646977</v>
+      </c>
+      <c r="G5">
+        <v>211.0257745378808</v>
+      </c>
+      <c r="H5">
+        <v>4823.98945779303</v>
+      </c>
+      <c r="I5">
+        <v>5258.521847420001</v>
+      </c>
+      <c r="J5">
+        <v>0.1526061066221148</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>123.75</v>
-      </c>
-      <c r="E4">
-        <v>49.75742447516642</v>
-      </c>
-      <c r="F4">
-        <v>53.54139368671829</v>
-      </c>
-      <c r="G4">
-        <v>2109.913629484222</v>
-      </c>
-      <c r="H4">
-        <v>1900.586950682596</v>
-      </c>
-      <c r="I4">
-        <v>0.4963474877610286</v>
-      </c>
-      <c r="J4">
-        <v>29.83333333333333</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>99.59999999999999</v>
-      </c>
-      <c r="E5">
-        <v>71.03225806451613</v>
-      </c>
-      <c r="F5">
-        <v>60.80704745666383</v>
-      </c>
-      <c r="G5">
-        <v>2109.913629484222</v>
-      </c>
-      <c r="H5">
-        <v>1900.586950682596</v>
-      </c>
-      <c r="I5">
-        <v>0.2574099493720388</v>
-      </c>
-      <c r="J5">
-        <v>29.83333333333333</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="M4" r:id="rId6"/>
-    <hyperlink ref="A5" r:id="rId7"/>
-    <hyperlink ref="M5" r:id="rId8"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="N3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="N4" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="N5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -958,17 +982,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
@@ -976,10 +1000,10 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1019,52 +1043,58 @@
       <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2">
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>858</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>30.51075268817204</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>226.272273699216</v>
-      </c>
-      <c r="G2">
-        <v>6788.168210976479</v>
       </c>
       <c r="H2">
         <v>6788.168210976479</v>
       </c>
       <c r="I2">
+        <v>6788.168210976479</v>
+      </c>
+      <c r="J2">
         <v>0.183959480597031</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>48.33333333333334</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>4</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1072,17 +1102,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
@@ -1090,10 +1120,10 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1133,52 +1163,58 @@
       <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2">
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>156.0909090909091</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>47.8289810547875</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>64.04526503871352</v>
-      </c>
-      <c r="G2">
-        <v>1921.357951161406</v>
       </c>
       <c r="H2">
         <v>1921.357951161406</v>
       </c>
       <c r="I2">
+        <v>1921.357951161406</v>
+      </c>
+      <c r="J2">
         <v>0.1334581662477377</v>
       </c>
-      <c r="J2">
-        <v>28.33333333333333</v>
-      </c>
       <c r="K2">
+        <v>27.66666666666667</v>
+      </c>
+      <c r="L2">
         <v>2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1186,17 +1222,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
@@ -1204,10 +1240,10 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1247,52 +1283,58 @@
       <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2">
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>191.7142857142857</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>72.73233486943165</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>120.9369522675062</v>
-      </c>
-      <c r="G2">
-        <v>3628.108568025185</v>
       </c>
       <c r="H2">
         <v>3628.108568025185</v>
       </c>
       <c r="I2">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="J2">
         <v>0.2311457247865123</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>33.16666666666666</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>3</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1300,17 +1342,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
@@ -1318,10 +1360,10 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1361,52 +1403,58 @@
       <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2">
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>191.7142857142857</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>72.73233486943165</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>120.9369522675062</v>
-      </c>
-      <c r="G2">
-        <v>3628.108568025185</v>
       </c>
       <c r="H2">
         <v>3628.108568025185</v>
       </c>
       <c r="I2">
+        <v>3628.108568025185</v>
+      </c>
+      <c r="J2">
         <v>0.4835642264939813</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>28.33333333333333</v>
-      </c>
-      <c r="K2">
-        <v>3</v>
       </c>
       <c r="L2">
         <v>3</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="N2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>